<commit_message>
add full state name to data
</commit_message>
<xml_diff>
--- a/data_tools/input/data.xlsx
+++ b/data_tools/input/data.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="25317"/>
   <workbookPr autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mhoyer\Documents\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2475" yWindow="1440" windowWidth="32025" windowHeight="25440" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="national_look" sheetId="1" r:id="rId1"/>
@@ -19,13 +14,13 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">local_lookup!$A$1:$T$140</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
     </ext>
   </extLst>
 </workbook>
@@ -952,9 +947,6 @@
     <t>GA</t>
   </si>
   <si>
-    <t>HA</t>
-  </si>
-  <si>
     <t>ID</t>
   </si>
   <si>
@@ -1103,6 +1095,9 @@
   </si>
   <si>
     <t>national_psychology</t>
+  </si>
+  <si>
+    <t>HI</t>
   </si>
 </sst>
 </file>
@@ -1461,7 +1456,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1475,15 +1470,15 @@
       <selection activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1497,7 +1492,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
@@ -1529,17 +1524,17 @@
       <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="28.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="1"/>
+    <col min="1" max="1" width="28.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" s="4" customFormat="1">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1559,7 +1554,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -1573,13 +1568,13 @@
         <v>43.4</v>
       </c>
       <c r="E2" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="F2">
         <v>51.7</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -1587,19 +1582,19 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D3">
         <v>34.200000000000003</v>
       </c>
       <c r="E3" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F3">
         <v>64.7</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4" t="s">
         <v>13</v>
       </c>
@@ -1607,19 +1602,19 @@
         <v>14</v>
       </c>
       <c r="C4" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D4">
         <v>32.200000000000003</v>
       </c>
       <c r="E4" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="F4">
         <v>52.5</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -1633,13 +1628,13 @@
         <v>31.900000000000002</v>
       </c>
       <c r="E5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F5">
         <v>39.5</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -1647,19 +1642,19 @@
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D6">
         <v>31.3</v>
       </c>
       <c r="E6" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="F6">
         <v>44.4</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7" t="s">
         <v>19</v>
       </c>
@@ -1667,19 +1662,19 @@
         <v>20</v>
       </c>
       <c r="C7" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D7">
         <v>31.1</v>
       </c>
       <c r="E7" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F7">
         <v>60</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -1687,19 +1682,19 @@
         <v>22</v>
       </c>
       <c r="C8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D8">
         <v>30.9</v>
       </c>
       <c r="E8" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="F8">
         <v>46.2</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -1713,13 +1708,13 @@
         <v>30.7</v>
       </c>
       <c r="E9" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F9">
         <v>44.800000000000004</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -1733,13 +1728,13 @@
         <v>30.3</v>
       </c>
       <c r="E10" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="F10">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11" t="s">
         <v>27</v>
       </c>
@@ -1747,13 +1742,13 @@
         <v>28</v>
       </c>
       <c r="C11" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D11">
         <v>29.5</v>
       </c>
       <c r="E11" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="F11">
         <v>87.1</v>
@@ -1774,30 +1769,30 @@
   <dimension ref="A1:T140"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R16" sqref="R16"/>
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="16" customWidth="1"/>
-    <col min="5" max="5" width="22.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22.140625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="24.140625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="25.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.140625" style="3" customWidth="1"/>
-    <col min="11" max="12" width="8.85546875" style="3"/>
-    <col min="13" max="13" width="17.42578125" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.42578125" style="3" customWidth="1"/>
-    <col min="15" max="16" width="8.85546875" style="3"/>
+    <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.1640625" style="16" customWidth="1"/>
+    <col min="5" max="5" width="22.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22.1640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.1640625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="25.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.1640625" style="3" customWidth="1"/>
+    <col min="11" max="12" width="8.83203125" style="3"/>
+    <col min="13" max="13" width="17.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.5" style="3" customWidth="1"/>
+    <col min="15" max="16" width="8.83203125" style="3"/>
     <col min="17" max="17" width="18" style="3" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="18" style="3" customWidth="1"/>
-    <col min="19" max="19" width="8.85546875" style="3"/>
+    <col min="19" max="19" width="8.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="9" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" s="9" customFormat="1">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1814,7 +1809,7 @@
         <v>30</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="G1" s="9" t="s">
         <v>2</v>
@@ -1826,40 +1821,40 @@
         <v>31</v>
       </c>
       <c r="J1" s="14" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="K1" s="12" t="s">
         <v>32</v>
       </c>
       <c r="L1" s="14" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="M1" s="12" t="s">
         <v>33</v>
       </c>
       <c r="N1" s="14" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="O1" s="12" t="s">
         <v>34</v>
       </c>
       <c r="P1" s="14" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="Q1" s="12" t="s">
         <v>35</v>
       </c>
       <c r="R1" s="14" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="S1" s="12" t="s">
         <v>36</v>
       </c>
       <c r="T1" s="17" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="2" spans="1:20">
       <c r="A2" t="s">
         <v>65</v>
       </c>
@@ -1921,7 +1916,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -1983,7 +1978,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20">
       <c r="A4" t="s">
         <v>267</v>
       </c>
@@ -2042,7 +2037,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20">
       <c r="A5" t="s">
         <v>37</v>
       </c>
@@ -2104,7 +2099,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20">
       <c r="A6" t="s">
         <v>193</v>
       </c>
@@ -2166,7 +2161,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20">
       <c r="A7" t="s">
         <v>211</v>
       </c>
@@ -2228,7 +2223,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20">
       <c r="A8" t="s">
         <v>245</v>
       </c>
@@ -2290,7 +2285,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20">
       <c r="A9" t="s">
         <v>77</v>
       </c>
@@ -2352,7 +2347,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20">
       <c r="A10" t="s">
         <v>132</v>
       </c>
@@ -2414,7 +2409,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20">
       <c r="A11" t="s">
         <v>79</v>
       </c>
@@ -2476,7 +2471,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20">
       <c r="A12" t="s">
         <v>126</v>
       </c>
@@ -2538,7 +2533,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20">
       <c r="A13" t="s">
         <v>155</v>
       </c>
@@ -2600,7 +2595,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20">
       <c r="A14" t="s">
         <v>15</v>
       </c>
@@ -2662,7 +2657,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:20">
       <c r="A15" t="s">
         <v>195</v>
       </c>
@@ -2724,7 +2719,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:20">
       <c r="A16" t="s">
         <v>207</v>
       </c>
@@ -2786,7 +2781,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:20">
       <c r="A17" t="s">
         <v>233</v>
       </c>
@@ -2848,7 +2843,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:20">
       <c r="A18" t="s">
         <v>235</v>
       </c>
@@ -2910,7 +2905,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:20">
       <c r="A19" t="s">
         <v>114</v>
       </c>
@@ -2972,7 +2967,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20">
       <c r="A20" t="s">
         <v>124</v>
       </c>
@@ -3034,7 +3029,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20">
       <c r="A21" t="s">
         <v>275</v>
       </c>
@@ -3096,7 +3091,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20">
       <c r="A22" t="s">
         <v>279</v>
       </c>
@@ -3158,7 +3153,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20">
       <c r="A23" t="s">
         <v>291</v>
       </c>
@@ -3217,7 +3212,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20">
       <c r="A24" t="s">
         <v>59</v>
       </c>
@@ -3279,7 +3274,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20">
       <c r="A25" t="s">
         <v>169</v>
       </c>
@@ -3341,7 +3336,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20">
       <c r="A26" t="s">
         <v>189</v>
       </c>
@@ -3403,7 +3398,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20">
       <c r="A27" t="s">
         <v>203</v>
       </c>
@@ -3465,7 +3460,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20">
       <c r="A28" t="s">
         <v>259</v>
       </c>
@@ -3527,7 +3522,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20">
       <c r="A29" t="s">
         <v>281</v>
       </c>
@@ -3589,7 +3584,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20">
       <c r="A30" t="s">
         <v>51</v>
       </c>
@@ -3651,7 +3646,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20">
       <c r="A31" t="s">
         <v>53</v>
       </c>
@@ -3713,7 +3708,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20">
       <c r="A32" t="s">
         <v>110</v>
       </c>
@@ -3775,7 +3770,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="33" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:20">
       <c r="A33" t="s">
         <v>205</v>
       </c>
@@ -3783,7 +3778,7 @@
         <v>206</v>
       </c>
       <c r="C33" t="s">
-        <v>306</v>
+        <v>356</v>
       </c>
       <c r="D33" s="16">
         <v>14708</v>
@@ -3834,7 +3829,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="34" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20">
       <c r="A34" t="s">
         <v>69</v>
       </c>
@@ -3842,7 +3837,7 @@
         <v>70</v>
       </c>
       <c r="C34" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D34" s="16">
         <v>15570</v>
@@ -3896,7 +3891,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:20">
       <c r="A35" t="s">
         <v>75</v>
       </c>
@@ -3904,7 +3899,7 @@
         <v>76</v>
       </c>
       <c r="C35" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D35" s="16">
         <v>15353</v>
@@ -3958,7 +3953,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:20">
       <c r="A36" t="s">
         <v>104</v>
       </c>
@@ -3966,7 +3961,7 @@
         <v>105</v>
       </c>
       <c r="C36" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D36" s="16">
         <v>19540</v>
@@ -4020,7 +4015,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="37" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:20">
       <c r="A37" t="s">
         <v>133</v>
       </c>
@@ -4028,7 +4023,7 @@
         <v>134</v>
       </c>
       <c r="C37" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D37" s="16">
         <v>55529</v>
@@ -4082,7 +4077,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:20">
       <c r="A38" t="s">
         <v>147</v>
       </c>
@@ -4090,7 +4085,7 @@
         <v>148</v>
       </c>
       <c r="C38" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D38" s="16">
         <v>43274</v>
@@ -4144,7 +4139,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:20">
       <c r="A39" t="s">
         <v>163</v>
       </c>
@@ -4152,7 +4147,7 @@
         <v>164</v>
       </c>
       <c r="C39" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D39" s="16">
         <v>24930</v>
@@ -4206,7 +4201,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:20">
       <c r="A40" t="s">
         <v>139</v>
       </c>
@@ -4214,7 +4209,7 @@
         <v>140</v>
       </c>
       <c r="C40" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D40" s="16">
         <v>54731</v>
@@ -4268,7 +4263,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:20">
       <c r="A41" t="s">
         <v>197</v>
       </c>
@@ -4276,7 +4271,7 @@
         <v>198</v>
       </c>
       <c r="C41" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D41" s="16">
         <v>32359</v>
@@ -4330,7 +4325,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:20">
       <c r="A42" t="s">
         <v>81</v>
       </c>
@@ -4338,7 +4333,7 @@
         <v>82</v>
       </c>
       <c r="C42" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D42" s="16">
         <v>18725</v>
@@ -4392,7 +4387,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20">
       <c r="A43" t="s">
         <v>141</v>
       </c>
@@ -4400,7 +4395,7 @@
         <v>142</v>
       </c>
       <c r="C43" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D43" s="16">
         <v>31750</v>
@@ -4454,7 +4449,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:20">
       <c r="A44" t="s">
         <v>116</v>
       </c>
@@ -4462,7 +4457,7 @@
         <v>117</v>
       </c>
       <c r="C44" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D44" s="16">
         <v>34135</v>
@@ -4516,7 +4511,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="45" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:20">
       <c r="A45" t="s">
         <v>287</v>
       </c>
@@ -4524,7 +4519,7 @@
         <v>288</v>
       </c>
       <c r="C45" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="D45" s="16">
         <v>17138</v>
@@ -4578,7 +4573,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="46" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:20">
       <c r="A46" t="s">
         <v>153</v>
       </c>
@@ -4586,7 +4581,7 @@
         <v>154</v>
       </c>
       <c r="C46" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D46" s="16">
         <v>34140</v>
@@ -4640,7 +4635,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:20">
       <c r="A47" t="s">
         <v>157</v>
       </c>
@@ -4648,7 +4643,7 @@
         <v>158</v>
       </c>
       <c r="C47" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="D47" s="16">
         <v>39707</v>
@@ -4702,7 +4697,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:20">
       <c r="A48" t="s">
         <v>41</v>
       </c>
@@ -4710,7 +4705,7 @@
         <v>42</v>
       </c>
       <c r="C48" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D48" s="16">
         <v>25300</v>
@@ -4764,7 +4759,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:20">
       <c r="A49" t="s">
         <v>239</v>
       </c>
@@ -4772,7 +4767,7 @@
         <v>240</v>
       </c>
       <c r="C49" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D49" s="16">
         <v>39812</v>
@@ -4826,7 +4821,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:20">
       <c r="A50" t="s">
         <v>27</v>
       </c>
@@ -4834,7 +4829,7 @@
         <v>28</v>
       </c>
       <c r="C50" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D50" s="16">
         <v>42627</v>
@@ -4888,7 +4883,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:20">
       <c r="A51" t="s">
         <v>63</v>
       </c>
@@ -4896,7 +4891,7 @@
         <v>64</v>
       </c>
       <c r="C51" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D51" s="16">
         <v>9214</v>
@@ -4947,7 +4942,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:20">
       <c r="A52" t="s">
         <v>269</v>
       </c>
@@ -4955,7 +4950,7 @@
         <v>270</v>
       </c>
       <c r="C52" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D52" s="16">
         <v>87383</v>
@@ -5009,7 +5004,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:20">
       <c r="A53" t="s">
         <v>273</v>
       </c>
@@ -5017,7 +5012,7 @@
         <v>274</v>
       </c>
       <c r="C53" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="D53" s="16">
         <v>24191</v>
@@ -5071,7 +5066,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:20">
       <c r="A54" t="s">
         <v>167</v>
       </c>
@@ -5079,7 +5074,7 @@
         <v>168</v>
       </c>
       <c r="C54" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="D54" s="16">
         <v>48763</v>
@@ -5133,7 +5128,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:20">
       <c r="A55" t="s">
         <v>23</v>
       </c>
@@ -5195,7 +5190,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:20">
       <c r="A56" t="s">
         <v>47</v>
       </c>
@@ -5203,7 +5198,7 @@
         <v>48</v>
       </c>
       <c r="C56" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D56" s="16">
         <v>50741</v>
@@ -5257,7 +5252,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:20">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -5265,7 +5260,7 @@
         <v>58</v>
       </c>
       <c r="C57" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D57" s="16">
         <v>21767</v>
@@ -5319,7 +5314,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:20">
       <c r="A58" t="s">
         <v>108</v>
       </c>
@@ -5327,7 +5322,7 @@
         <v>109</v>
       </c>
       <c r="C58" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D58" s="16">
         <v>40763</v>
@@ -5381,7 +5376,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:20">
       <c r="A59" t="s">
         <v>143</v>
       </c>
@@ -5389,7 +5384,7 @@
         <v>144</v>
       </c>
       <c r="C59" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D59" s="16">
         <v>13041</v>
@@ -5443,7 +5438,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:20">
       <c r="A60" t="s">
         <v>225</v>
       </c>
@@ -5451,7 +5446,7 @@
         <v>226</v>
       </c>
       <c r="C60" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D60" s="16">
         <v>23265</v>
@@ -5505,7 +5500,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:20">
       <c r="A61" t="s">
         <v>173</v>
       </c>
@@ -5513,7 +5508,7 @@
         <v>174</v>
       </c>
       <c r="C61" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D61" s="16">
         <v>72238</v>
@@ -5567,7 +5562,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:20">
       <c r="A62" t="s">
         <v>253</v>
       </c>
@@ -5575,7 +5570,7 @@
         <v>254</v>
       </c>
       <c r="C62" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="D62" s="16">
         <v>33773</v>
@@ -5629,7 +5624,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:20">
       <c r="A63" t="s">
         <v>128</v>
       </c>
@@ -5637,7 +5632,7 @@
         <v>129</v>
       </c>
       <c r="C63" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D63" s="16">
         <v>47847</v>
@@ -5691,7 +5686,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:20">
       <c r="A64" t="s">
         <v>145</v>
       </c>
@@ -5699,7 +5694,7 @@
         <v>146</v>
       </c>
       <c r="C64" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="D64" s="16">
         <v>38039</v>
@@ -5753,7 +5748,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20">
       <c r="A65" t="s">
         <v>99</v>
       </c>
@@ -5761,7 +5756,7 @@
         <v>100</v>
       </c>
       <c r="C65" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D65" s="16">
         <v>30608</v>
@@ -5815,7 +5810,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20">
       <c r="A66" t="s">
         <v>149</v>
       </c>
@@ -5823,7 +5818,7 @@
         <v>150</v>
       </c>
       <c r="C66" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D66" s="16">
         <v>33271</v>
@@ -5877,7 +5872,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20">
       <c r="A67" t="s">
         <v>215</v>
       </c>
@@ -5885,7 +5880,7 @@
         <v>216</v>
       </c>
       <c r="C67" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D67" s="16">
         <v>11620</v>
@@ -5939,7 +5934,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20">
       <c r="A68" t="s">
         <v>255</v>
       </c>
@@ -5947,7 +5942,7 @@
         <v>256</v>
       </c>
       <c r="C68" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="D68" s="16">
         <v>45658</v>
@@ -6001,7 +5996,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20">
       <c r="A69" t="s">
         <v>175</v>
       </c>
@@ -6009,7 +6004,7 @@
         <v>176</v>
       </c>
       <c r="C69" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="D69" s="16">
         <v>18714</v>
@@ -6063,7 +6058,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20">
       <c r="A70" t="s">
         <v>49</v>
       </c>
@@ -6071,7 +6066,7 @@
         <v>50</v>
       </c>
       <c r="C70" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D70" s="16">
         <v>40653</v>
@@ -6125,7 +6120,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20">
       <c r="A71" t="s">
         <v>112</v>
       </c>
@@ -6133,7 +6128,7 @@
         <v>113</v>
       </c>
       <c r="C71" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D71" s="16">
         <v>65725</v>
@@ -6187,7 +6182,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20">
       <c r="A72" t="s">
         <v>13</v>
       </c>
@@ -6195,7 +6190,7 @@
         <v>14</v>
       </c>
       <c r="C72" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D72" s="16">
         <v>42689</v>
@@ -6249,7 +6244,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20">
       <c r="A73" t="s">
         <v>229</v>
       </c>
@@ -6257,7 +6252,7 @@
         <v>230</v>
       </c>
       <c r="C73" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D73" s="16">
         <v>76063</v>
@@ -6311,7 +6306,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:20">
       <c r="A74" t="s">
         <v>122</v>
       </c>
@@ -6319,7 +6314,7 @@
         <v>123</v>
       </c>
       <c r="C74" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="D74" s="16">
         <v>20216</v>
@@ -6373,7 +6368,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:20">
       <c r="A75" t="s">
         <v>161</v>
       </c>
@@ -6381,7 +6376,7 @@
         <v>162</v>
       </c>
       <c r="C75" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="D75" s="16">
         <v>21750</v>
@@ -6435,7 +6430,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:20">
       <c r="A76" t="s">
         <v>183</v>
       </c>
@@ -6443,7 +6438,7 @@
         <v>184</v>
       </c>
       <c r="C76" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="D76" s="16">
         <v>39672</v>
@@ -6497,7 +6492,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:20">
       <c r="A77" t="s">
         <v>185</v>
       </c>
@@ -6505,7 +6500,7 @@
         <v>186</v>
       </c>
       <c r="C77" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="D77" s="16">
         <v>47254</v>
@@ -6559,7 +6554,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:20">
       <c r="A78" t="s">
         <v>39</v>
       </c>
@@ -6567,7 +6562,7 @@
         <v>40</v>
       </c>
       <c r="C78" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D78" s="16">
         <v>30341</v>
@@ -6621,7 +6616,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:20">
       <c r="A79" t="s">
         <v>55</v>
       </c>
@@ -6629,7 +6624,7 @@
         <v>56</v>
       </c>
       <c r="C79" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D79" s="16">
         <v>17431</v>
@@ -6680,7 +6675,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:20">
       <c r="A80" t="s">
         <v>71</v>
       </c>
@@ -6688,7 +6683,7 @@
         <v>72</v>
       </c>
       <c r="C80" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D80" s="16">
         <v>25353</v>
@@ -6739,7 +6734,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:20">
       <c r="A81" t="s">
         <v>73</v>
       </c>
@@ -6747,7 +6742,7 @@
         <v>74</v>
       </c>
       <c r="C81" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D81" s="16">
         <v>14055</v>
@@ -6801,7 +6796,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:20">
       <c r="A82" t="s">
         <v>187</v>
       </c>
@@ -6809,7 +6804,7 @@
         <v>188</v>
       </c>
       <c r="C82" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D82" s="16">
         <v>44488</v>
@@ -6863,7 +6858,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:20">
       <c r="A83" t="s">
         <v>199</v>
       </c>
@@ -6871,7 +6866,7 @@
         <v>200</v>
       </c>
       <c r="C83" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D83" s="16">
         <v>33696</v>
@@ -6925,7 +6920,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:20">
       <c r="A84" t="s">
         <v>257</v>
       </c>
@@ -6933,7 +6928,7 @@
         <v>258</v>
       </c>
       <c r="C84" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D84" s="16">
         <v>44241</v>
@@ -6987,7 +6982,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:20">
       <c r="A85" t="s">
         <v>277</v>
       </c>
@@ -6995,7 +6990,7 @@
         <v>278</v>
       </c>
       <c r="C85" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D85" s="16">
         <v>21061</v>
@@ -7049,7 +7044,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:20">
       <c r="A86" t="s">
         <v>283</v>
       </c>
@@ -7057,7 +7052,7 @@
         <v>284</v>
       </c>
       <c r="C86" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D86" s="16">
         <v>43953</v>
@@ -7111,7 +7106,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:20">
       <c r="A87" t="s">
         <v>181</v>
       </c>
@@ -7119,7 +7114,7 @@
         <v>182</v>
       </c>
       <c r="C87" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D87" s="16">
         <v>37172</v>
@@ -7173,7 +7168,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:20">
       <c r="A88" t="s">
         <v>21</v>
       </c>
@@ -7181,7 +7176,7 @@
         <v>22</v>
       </c>
       <c r="C88" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D88" s="16">
         <v>26131</v>
@@ -7235,7 +7230,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:20">
       <c r="A89" t="s">
         <v>247</v>
       </c>
@@ -7243,7 +7238,7 @@
         <v>248</v>
       </c>
       <c r="C89" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="D89" s="16">
         <v>61449</v>
@@ -7297,7 +7292,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:20">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -7305,7 +7300,7 @@
         <v>90</v>
       </c>
       <c r="C90" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D90" s="16">
         <v>15651</v>
@@ -7359,7 +7354,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:20">
       <c r="A91" t="s">
         <v>91</v>
       </c>
@@ -7367,7 +7362,7 @@
         <v>92</v>
       </c>
       <c r="C91" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D91" s="16">
         <v>40545</v>
@@ -7421,7 +7416,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:20">
       <c r="A92" t="s">
         <v>95</v>
       </c>
@@ -7429,7 +7424,7 @@
         <v>96</v>
       </c>
       <c r="C92" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D92" s="16">
         <v>81928</v>
@@ -7483,7 +7478,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:20">
       <c r="A93" t="s">
         <v>102</v>
       </c>
@@ -7491,7 +7486,7 @@
         <v>103</v>
       </c>
       <c r="C93" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D93" s="16">
         <v>37736</v>
@@ -7545,7 +7540,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:20">
       <c r="A94" t="s">
         <v>106</v>
       </c>
@@ -7553,7 +7548,7 @@
         <v>107</v>
       </c>
       <c r="C94" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="D94" s="16">
         <v>26159</v>
@@ -7607,7 +7602,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:20">
       <c r="A95" t="s">
         <v>179</v>
       </c>
@@ -7615,7 +7610,7 @@
         <v>180</v>
       </c>
       <c r="C95" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D95" s="16">
         <v>23567</v>
@@ -7669,7 +7664,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:20">
       <c r="A96" t="s">
         <v>201</v>
       </c>
@@ -7677,7 +7672,7 @@
         <v>202</v>
       </c>
       <c r="C96" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D96" s="16">
         <v>38763</v>
@@ -7731,7 +7726,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:20">
       <c r="A97" t="s">
         <v>217</v>
       </c>
@@ -7739,7 +7734,7 @@
         <v>218</v>
       </c>
       <c r="C97" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D97" s="16">
         <v>75690</v>
@@ -7793,7 +7788,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:20">
       <c r="A98" t="s">
         <v>11</v>
       </c>
@@ -7801,7 +7796,7 @@
         <v>12</v>
       </c>
       <c r="C98" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D98" s="16">
         <v>21078</v>
@@ -7855,7 +7850,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:20">
       <c r="A99" t="s">
         <v>249</v>
       </c>
@@ -7863,7 +7858,7 @@
         <v>250</v>
       </c>
       <c r="C99" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="D99" s="16">
         <v>11069</v>
@@ -7917,7 +7912,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:20">
       <c r="A100" t="s">
         <v>43</v>
       </c>
@@ -7925,7 +7920,7 @@
         <v>44</v>
       </c>
       <c r="C100" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D100" s="16">
         <v>30541</v>
@@ -7979,7 +7974,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:20">
       <c r="A101" t="s">
         <v>97</v>
       </c>
@@ -7987,7 +7982,7 @@
         <v>98</v>
       </c>
       <c r="C101" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D101" s="16">
         <v>9373</v>
@@ -8041,7 +8036,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:20">
       <c r="A102" t="s">
         <v>120</v>
       </c>
@@ -8049,7 +8044,7 @@
         <v>121</v>
       </c>
       <c r="C102" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D102" s="16">
         <v>14888</v>
@@ -8103,7 +8098,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:20">
       <c r="A103" t="s">
         <v>151</v>
       </c>
@@ -8111,7 +8106,7 @@
         <v>152</v>
       </c>
       <c r="C103" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D103" s="16">
         <v>54288</v>
@@ -8165,7 +8160,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:20">
       <c r="A104" t="s">
         <v>209</v>
       </c>
@@ -8173,7 +8168,7 @@
         <v>210</v>
       </c>
       <c r="C104" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D104" s="16">
         <v>62197</v>
@@ -8227,7 +8222,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:20">
       <c r="A105" t="s">
         <v>213</v>
       </c>
@@ -8235,7 +8230,7 @@
         <v>214</v>
       </c>
       <c r="C105" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D105" s="16">
         <v>57393</v>
@@ -8289,7 +8284,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:20">
       <c r="A106" t="s">
         <v>271</v>
       </c>
@@ -8297,7 +8292,7 @@
         <v>272</v>
       </c>
       <c r="C106" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D106" s="16">
         <v>24323</v>
@@ -8351,7 +8346,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:20">
       <c r="A107" t="s">
         <v>289</v>
       </c>
@@ -8359,7 +8354,7 @@
         <v>290</v>
       </c>
       <c r="C107" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="D107" s="16">
         <v>28408</v>
@@ -8413,7 +8408,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:20">
       <c r="A108" t="s">
         <v>219</v>
       </c>
@@ -8421,7 +8416,7 @@
         <v>220</v>
       </c>
       <c r="C108" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D108" s="16">
         <v>43359</v>
@@ -8475,7 +8470,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:20">
       <c r="A109" t="s">
         <v>85</v>
       </c>
@@ -8483,7 +8478,7 @@
         <v>86</v>
       </c>
       <c r="C109" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D109" s="16">
         <v>48662</v>
@@ -8537,7 +8532,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:20">
       <c r="A110" t="s">
         <v>101</v>
       </c>
@@ -8545,7 +8540,7 @@
         <v>100</v>
       </c>
       <c r="C110" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="D110" s="16">
         <v>57331</v>
@@ -8599,7 +8594,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:20">
       <c r="A111" t="s">
         <v>67</v>
       </c>
@@ -8607,7 +8602,7 @@
         <v>68</v>
       </c>
       <c r="C111" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D111" s="16">
         <v>13381</v>
@@ -8661,7 +8656,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:20">
       <c r="A112" t="s">
         <v>241</v>
       </c>
@@ -8669,7 +8664,7 @@
         <v>242</v>
       </c>
       <c r="C112" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="D112" s="16">
         <v>21456</v>
@@ -8723,7 +8718,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:20">
       <c r="A113" t="s">
         <v>19</v>
       </c>
@@ -8731,7 +8726,7 @@
         <v>20</v>
       </c>
       <c r="C113" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D113" s="16">
         <v>57402</v>
@@ -8785,7 +8780,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:20">
       <c r="A114" t="s">
         <v>177</v>
       </c>
@@ -8793,7 +8788,7 @@
         <v>178</v>
       </c>
       <c r="C114" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D114" s="16">
         <v>81397</v>
@@ -8847,7 +8842,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:20">
       <c r="A115" t="s">
         <v>261</v>
       </c>
@@ -8855,7 +8850,7 @@
         <v>262</v>
       </c>
       <c r="C115" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="D115" s="16">
         <v>132258</v>
@@ -8909,7 +8904,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:20">
       <c r="A116" t="s">
         <v>45</v>
       </c>
@@ -8971,7 +8966,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:20">
       <c r="A117" t="s">
         <v>83</v>
       </c>
@@ -9033,7 +9028,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:20">
       <c r="A118" t="s">
         <v>118</v>
       </c>
@@ -9095,7 +9090,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:20">
       <c r="A119" t="s">
         <v>135</v>
       </c>
@@ -9157,7 +9152,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:20">
       <c r="A120" t="s">
         <v>191</v>
       </c>
@@ -9219,7 +9214,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:20">
       <c r="A121" t="s">
         <v>243</v>
       </c>
@@ -9281,7 +9276,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:20">
       <c r="A122" t="s">
         <v>263</v>
       </c>
@@ -9343,7 +9338,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:20">
       <c r="A123" t="s">
         <v>9</v>
       </c>
@@ -9402,7 +9397,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:20">
       <c r="A124" t="s">
         <v>231</v>
       </c>
@@ -9410,7 +9405,7 @@
         <v>232</v>
       </c>
       <c r="C124" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="D124" s="16">
         <v>29517</v>
@@ -9464,7 +9459,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:20">
       <c r="A125" t="s">
         <v>130</v>
       </c>
@@ -9472,7 +9467,7 @@
         <v>131</v>
       </c>
       <c r="C125" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D125" s="16">
         <v>38401</v>
@@ -9526,7 +9521,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:20">
       <c r="A126" t="s">
         <v>223</v>
       </c>
@@ -9534,7 +9529,7 @@
         <v>224</v>
       </c>
       <c r="C126" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D126" s="16">
         <v>69708</v>
@@ -9588,7 +9583,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:20">
       <c r="A127" t="s">
         <v>227</v>
       </c>
@@ -9596,7 +9591,7 @@
         <v>228</v>
       </c>
       <c r="C127" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="D127" s="16">
         <v>42131</v>
@@ -9650,7 +9645,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:20">
       <c r="A128" t="s">
         <v>285</v>
       </c>
@@ -9658,7 +9653,7 @@
         <v>286</v>
       </c>
       <c r="C128" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="D128" s="16">
         <v>21256</v>
@@ -9712,7 +9707,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:20">
       <c r="A129" t="s">
         <v>61</v>
       </c>
@@ -9720,7 +9715,7 @@
         <v>62</v>
       </c>
       <c r="C129" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D129" s="16">
         <v>15471</v>
@@ -9774,7 +9769,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:20">
       <c r="A130" t="s">
         <v>93</v>
       </c>
@@ -9782,7 +9777,7 @@
         <v>94</v>
       </c>
       <c r="C130" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D130" s="16">
         <v>25047</v>
@@ -9836,7 +9831,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:20">
       <c r="A131" t="s">
         <v>137</v>
       </c>
@@ -9844,7 +9839,7 @@
         <v>138</v>
       </c>
       <c r="C131" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D131" s="16">
         <v>28566</v>
@@ -9898,7 +9893,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:20">
       <c r="A132" t="s">
         <v>165</v>
       </c>
@@ -9906,7 +9901,7 @@
         <v>166</v>
       </c>
       <c r="C132" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D132" s="16">
         <v>35985</v>
@@ -9960,7 +9955,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:20">
       <c r="A133" t="s">
         <v>221</v>
       </c>
@@ -9968,7 +9963,7 @@
         <v>222</v>
       </c>
       <c r="C133" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D133" s="16">
         <v>67504</v>
@@ -10022,7 +10017,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:20">
       <c r="A134" t="s">
         <v>251</v>
       </c>
@@ -10030,7 +10025,7 @@
         <v>252</v>
       </c>
       <c r="C134" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D134" s="16">
         <v>21432</v>
@@ -10084,7 +10079,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:20">
       <c r="A135" t="s">
         <v>17</v>
       </c>
@@ -10092,7 +10087,7 @@
         <v>18</v>
       </c>
       <c r="C135" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="D135" s="16">
         <v>7946</v>
@@ -10146,7 +10141,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:20">
       <c r="A136" t="s">
         <v>159</v>
       </c>
@@ -10154,7 +10149,7 @@
         <v>160</v>
       </c>
       <c r="C136" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D136" s="16">
         <v>31479</v>
@@ -10208,7 +10203,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:20">
       <c r="A137" t="s">
         <v>171</v>
       </c>
@@ -10216,7 +10211,7 @@
         <v>172</v>
       </c>
       <c r="C137" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D137" s="16">
         <v>55523</v>
@@ -10270,7 +10265,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:20">
       <c r="A138" t="s">
         <v>265</v>
       </c>
@@ -10278,7 +10273,7 @@
         <v>266</v>
       </c>
       <c r="C138" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="D138" s="16">
         <v>14532</v>
@@ -10332,7 +10327,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:20">
       <c r="A139" t="s">
         <v>87</v>
       </c>
@@ -10340,7 +10335,7 @@
         <v>88</v>
       </c>
       <c r="C139" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D139" s="16">
         <v>14039</v>
@@ -10391,7 +10386,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="140" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:20">
       <c r="A140" t="s">
         <v>237</v>
       </c>
@@ -10399,7 +10394,7 @@
         <v>238</v>
       </c>
       <c r="C140" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="D140" s="16">
         <v>4105</v>

</xml_diff>